<commit_message>
fix field naming issues
</commit_message>
<xml_diff>
--- a/Forms/ReportTemplates/History Taking (Page 2).xlsx
+++ b/Forms/ReportTemplates/History Taking (Page 2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\i2emr\Forms\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917A6FDB-09DF-4149-A7A4-1FC3BFB763E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A3F710-DEDC-4AD8-9B14-A54A69BB9E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75CF79CF-7F7D-4998-9773-FADB7D42A4C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75CF79CF-7F7D-4998-9773-FADB7D42A4C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,75 +38,6 @@
     <t>Hx NSS</t>
   </si>
   <si>
-    <t>hxHssQ1</t>
-  </si>
-  <si>
-    <t>hxHssQ2</t>
-  </si>
-  <si>
-    <t>hxHssQ3</t>
-  </si>
-  <si>
-    <t>hxHssQ4</t>
-  </si>
-  <si>
-    <t>hxHssQ5</t>
-  </si>
-  <si>
-    <t>hxHssQ6</t>
-  </si>
-  <si>
-    <t>hxHssQ7</t>
-  </si>
-  <si>
-    <t>hxHssQ8</t>
-  </si>
-  <si>
-    <t>hxHssQ9</t>
-  </si>
-  <si>
-    <t>hxHssQ10</t>
-  </si>
-  <si>
-    <t>hxHssQ11</t>
-  </si>
-  <si>
-    <t>hxHssQ12</t>
-  </si>
-  <si>
-    <t>hxHssQ13</t>
-  </si>
-  <si>
-    <t>hxHssQ14</t>
-  </si>
-  <si>
-    <t>hxHssQ15</t>
-  </si>
-  <si>
-    <t>hxHssQ16</t>
-  </si>
-  <si>
-    <t>hxHssQ17</t>
-  </si>
-  <si>
-    <t>hxHssQ18</t>
-  </si>
-  <si>
-    <t>hxHssQ19</t>
-  </si>
-  <si>
-    <t>hxHssQ20</t>
-  </si>
-  <si>
-    <t>hxHssQ21</t>
-  </si>
-  <si>
-    <t>hxHssQ22</t>
-  </si>
-  <si>
-    <t>hxHssQ23</t>
-  </si>
-  <si>
     <t>1a. Has a doctor ever told you that you have the following condition?</t>
   </si>
   <si>
@@ -131,9 +62,6 @@
     <t>2c. Are you currently being prescribed any medication for any of the conditions below? Stroke</t>
   </si>
   <si>
-    <t>hxHssQ24</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please tick to highlight if you feel BLOOD PRESSURE requires closer scrutiny by doctors later </t>
   </si>
   <si>
@@ -171,6 +99,78 @@
   </si>
   <si>
     <t>9. Has your doctor told you that the blood vessels to your limbs are diseased and have become narrower (periphery artery disease) or that any other major blood vessels in your body have weakened walls that have "ballooned out" (aneurysm)?</t>
+  </si>
+  <si>
+    <t>hxNssQ1</t>
+  </si>
+  <si>
+    <t>hxNssQ2</t>
+  </si>
+  <si>
+    <t>hxNssQ3</t>
+  </si>
+  <si>
+    <t>hxNssQ4</t>
+  </si>
+  <si>
+    <t>hxNssQ22</t>
+  </si>
+  <si>
+    <t>hxNssQ5</t>
+  </si>
+  <si>
+    <t>hxNssQ6</t>
+  </si>
+  <si>
+    <t>hxNssQ7</t>
+  </si>
+  <si>
+    <t>hxNssQ8</t>
+  </si>
+  <si>
+    <t>hxNssQ24</t>
+  </si>
+  <si>
+    <t>hxNssQ9</t>
+  </si>
+  <si>
+    <t>hxNssQ10</t>
+  </si>
+  <si>
+    <t>hxNssQ11</t>
+  </si>
+  <si>
+    <t>hxNssQ12</t>
+  </si>
+  <si>
+    <t>hxNssQ13</t>
+  </si>
+  <si>
+    <t>hxNssQ23</t>
+  </si>
+  <si>
+    <t>hxNssQ14</t>
+  </si>
+  <si>
+    <t>hxNssQ15</t>
+  </si>
+  <si>
+    <t>hxNssQ16</t>
+  </si>
+  <si>
+    <t>hxNssQ17</t>
+  </si>
+  <si>
+    <t>hxNssQ18</t>
+  </si>
+  <si>
+    <t>hxNssQ19</t>
+  </si>
+  <si>
+    <t>hxNssQ20</t>
+  </si>
+  <si>
+    <t>hxNssQ21</t>
   </si>
 </sst>
 </file>
@@ -533,186 +533,186 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC5F2F1-36A0-4965-BAA8-67364BD15367}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" customWidth="1"/>
-    <col min="8" max="9" width="22.28515625" customWidth="1"/>
-    <col min="10" max="11" width="27.140625" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="14" width="22.28515625" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" customWidth="1"/>
-    <col min="18" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="26" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="11" width="27.109375" customWidth="1"/>
+    <col min="12" max="12" width="27.33203125" customWidth="1"/>
+    <col min="13" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="18" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="26" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="N2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="O2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="R2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="S2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="T2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="U2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="V2" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="W2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="X2" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="Y2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="1" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="1" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>